<commit_message>
First draft, missing final results
</commit_message>
<xml_diff>
--- a/Tables/Link Budget.xlsx
+++ b/Tables/Link Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fredrikfeyling/Documents/Skole/V20/Radio/Project Report/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05F1695-F25E-8848-8E4D-006E0B432A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35ADBC7-5356-DA41-B9C5-6CD5AB30B3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16040" xr2:uid="{D23B0FDC-2720-5246-BF19-F622F0F7BB99}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" xr2:uid="{D23B0FDC-2720-5246-BF19-F622F0F7BB99}"/>
   </bookViews>
   <sheets>
     <sheet name="Link Budget" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>Variable</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>Eb over N0</t>
-  </si>
-  <si>
-    <t>lin</t>
   </si>
   <si>
     <t>BER</t>
@@ -358,17 +355,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -377,45 +409,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,17 +734,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C91FB6-C9A7-7E44-9EDC-C51A06F5BF27}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="28.6640625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="19" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" style="1" customWidth="1"/>
   </cols>
@@ -762,24 +759,24 @@
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" ht="17">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -792,11 +789,11 @@
       <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="8">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="21">
+        <v>-10</v>
+      </c>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
@@ -808,13 +805,13 @@
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="22">
         <v>-0.3</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6" ht="17">
       <c r="A5" s="5" t="s">
@@ -826,14 +823,14 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="21">
         <f>E3+2*E4</f>
-        <v>9.4</v>
-      </c>
-      <c r="F5" s="8"/>
+        <v>-10.6</v>
+      </c>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
@@ -845,13 +842,13 @@
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="D6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="21">
         <v>3</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="5" t="s">
@@ -863,22 +860,22 @@
       <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="D7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="21">
         <f>E5+E6</f>
-        <v>12.4</v>
-      </c>
-      <c r="F7" s="8"/>
+        <v>-7.6</v>
+      </c>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
     </row>
@@ -892,11 +889,11 @@
       <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="8">
-        <v>10</v>
-      </c>
-      <c r="F9" s="8"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="21">
+        <v>2</v>
+      </c>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
@@ -908,11 +905,11 @@
       <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="8">
+      <c r="D10" s="14"/>
+      <c r="E10" s="21">
         <v>0</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
@@ -922,11 +919,11 @@
         <v>34</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="8">
+      <c r="D11" s="14"/>
+      <c r="E11" s="21">
         <v>38</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
@@ -938,12 +935,12 @@
       <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="27">
+      <c r="D12" s="14"/>
+      <c r="E12" s="24">
         <f>-(20*LOG10(2415)+E11*LOG10(E9)-28+E10)</f>
-        <v>-77.658342701750612</v>
-      </c>
-      <c r="F12" s="27"/>
+        <v>-51.0974825369819</v>
+      </c>
+      <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
@@ -951,7 +948,7 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
     </row>
@@ -965,12 +962,12 @@
       <c r="C14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="8">
+      <c r="D14" s="14"/>
+      <c r="E14" s="21">
         <f>E6</f>
         <v>3</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
@@ -982,12 +979,12 @@
       <c r="C15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="8">
+      <c r="D15" s="14"/>
+      <c r="E15" s="21">
         <f>E4</f>
         <v>-0.3</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
@@ -999,20 +996,20 @@
       <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="8">
+      <c r="D16" s="14"/>
+      <c r="E16" s="21">
         <f>E14+E15*2</f>
         <v>2.4</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" ht="34">
       <c r="A18" s="5" t="s">
@@ -1024,14 +1021,14 @@
       <c r="C18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="27">
         <f>E7+E12+E16</f>
-        <v>-62.858342701750608</v>
-      </c>
-      <c r="F18" s="28"/>
+        <v>-56.297482536981903</v>
+      </c>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
@@ -1039,90 +1036,90 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="20"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="30">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="28">
         <v>-145.72999999999999</v>
       </c>
-      <c r="F20" s="11"/>
+      <c r="F20" s="28"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="25">
         <f>10*LOG10(10^(E20/10)*62*1000)</f>
         <v>-97.806083105017464</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="25">
         <v>7</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:6" ht="30">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="25">
         <v>9.4</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
     </row>
@@ -1131,111 +1128,91 @@
         <v>47</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="13">
+      <c r="D25" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="26">
         <f>E18-E21-E22-E23</f>
-        <v>18.547740403266857</v>
-      </c>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" ht="51">
+        <v>25.108600568035563</v>
+      </c>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="1:6" ht="34">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="14">
+      <c r="D26" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="9">
         <f>E25-10*LOG10(187.39/60.9)</f>
-        <v>13.666449217583716</v>
-      </c>
-      <c r="F26" s="14">
+        <v>20.227309382352423</v>
+      </c>
+      <c r="F26" s="9">
         <f>E25-10*LOG10(572.67/62)</f>
-        <v>8.8926129714939037</v>
+        <v>15.453473136262609</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="14">
-        <f>10^(E26/10)</f>
-        <v>23.261885931340604</v>
-      </c>
-      <c r="F27" s="14">
-        <f>10^(F26/10)</f>
-        <v>7.749278998553307</v>
+      <c r="C27" s="6"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="10">
+        <f>0.5*ERFC(SQRT(E26))</f>
+        <v>1.0061808764039024E-10</v>
+      </c>
+      <c r="F27" s="11">
+        <f>2/LOG(64, 2)*(1-1/SQRT(64))*ERFC(SQRT(3*LOG(64,2)/(2*15)*F26))</f>
+        <v>4.8420284952290429E-6</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="16">
-        <f>0.5*ERFC(SQRT(E26))</f>
-        <v>8.5636248466390753E-8</v>
-      </c>
-      <c r="F28" s="17">
-        <f>2/LOG(64, 2)*(1-1/SQRT(64))*ERFC(SQRT(3*LOG(64,2)/(2*15)*F26))</f>
-        <v>3.1739251781031421E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>